<commit_message>
Took away some required fields in the farm interview
</commit_message>
<xml_diff>
--- a/forms/psa_farm_interview/psa_farm_interview.xlsx
+++ b/forms/psa_farm_interview/psa_farm_interview.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saseehav\Documents\GitHub\Kobo\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saseehav\Documents\GitHub\Kobo\forms\psa_farm_interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -122,13 +122,16 @@
     <t>If a grower has multiple trial fields, the survey will automatically prompt you to enter data for the additional fields; thus you only need to complete one survey per grower.  You will need to know the 3-letter trial code(s) associated with each trial field.</t>
   </si>
   <si>
+    <t>noteswipe</t>
+  </si>
+  <si>
     <t>Swipe left for the first group of questions.       If you arrive at the end of a group, and are not prompted to Submit, swipe left.</t>
   </si>
   <si>
     <t>group_ct2kn52</t>
   </si>
   <si>
-    <t xml:space="preserve">Technician and Farmer Contact Information </t>
+    <t>Technician and Farmer Contact Information</t>
   </si>
   <si>
     <t>text</t>
@@ -140,33 +143,33 @@
     <t>1. State [please enter the two-letter abbreviation for your state, example: NC]</t>
   </si>
   <si>
+    <t>tech</t>
+  </si>
+  <si>
+    <t>2. Field tech last name</t>
+  </si>
+  <si>
+    <t>tech_phone</t>
+  </si>
+  <si>
+    <t>3. Field tech phone number</t>
+  </si>
+  <si>
+    <t>tech_email</t>
+  </si>
+  <si>
+    <t>4. Field tech email</t>
+  </si>
+  <si>
+    <t>grower_last_name</t>
+  </si>
+  <si>
+    <t>5. Grower last name</t>
+  </si>
+  <si>
     <t>true</t>
   </si>
   <si>
-    <t>tech</t>
-  </si>
-  <si>
-    <t>2. Field tech last name</t>
-  </si>
-  <si>
-    <t>tech_phone</t>
-  </si>
-  <si>
-    <t>3. Field tech phone number</t>
-  </si>
-  <si>
-    <t>tech_email</t>
-  </si>
-  <si>
-    <t>4. Field tech email</t>
-  </si>
-  <si>
-    <t>grower_last_name</t>
-  </si>
-  <si>
-    <t>5. Grower last name</t>
-  </si>
-  <si>
     <t>grower_phone</t>
   </si>
   <si>
@@ -182,477 +185,516 @@
     <t>select_one yy77y77</t>
   </si>
   <si>
+    <t>farm_or_station</t>
+  </si>
+  <si>
     <t>Is this a farm or research station? (If this is a research station, you will skip the farmer interview portion and go directly to site history information.)</t>
   </si>
   <si>
+    <t>group_social_sci_survey</t>
+  </si>
+  <si>
+    <t>General Whole Farm Survey</t>
+  </si>
+  <si>
+    <t>${farm_or_station} = 'farm'</t>
+  </si>
+  <si>
+    <t>note5</t>
+  </si>
+  <si>
+    <t>Please have the grower respond to the questions that follow.</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>crop_acres</t>
+  </si>
+  <si>
+    <t>8. As of today, how many total acres do you plant in crops? [acres]</t>
+  </si>
+  <si>
+    <t>select_multiple dq65c45</t>
+  </si>
+  <si>
+    <t>farm_crop_rotation</t>
+  </si>
+  <si>
+    <t>9. What crops are GENERALLY in your crop rotation?</t>
+  </si>
+  <si>
+    <t>cover_crop_acres</t>
+  </si>
+  <si>
+    <t>10. As of today, how many of your total cropped acres are in COVER CROPS? [acres]</t>
+  </si>
+  <si>
+    <t>cover_crop_acres_terminated</t>
+  </si>
+  <si>
+    <t>10.a Clarification:  If COVER CROPS have already been terminated, how many acres did you have of winter cover crops prior to termination? [# acres, or leave blank if not applicable]</t>
+  </si>
+  <si>
+    <t>${cover_crop_acres} = 0</t>
+  </si>
+  <si>
+    <t>cover_crop_acres_typical</t>
+  </si>
+  <si>
+    <t>11.  If this was a particularly bad or otherwise non-representative year, how many acres do you typically have of winter COVER CROPS?  [# acres, or leave blank if not applicable]</t>
+  </si>
+  <si>
+    <t>first_year_cover_crop</t>
+  </si>
+  <si>
+    <t>12. In what year did you first plant COVER CROPS? [four digit year, example : 1985] *reminder, for a grower to participate, this may not be their first time planting cover crops</t>
+  </si>
+  <si>
+    <t>select_one xe2wp37</t>
+  </si>
+  <si>
+    <t>every_year</t>
+  </si>
+  <si>
+    <t>13. Have you planted COVER CROPS every year since?</t>
+  </si>
+  <si>
+    <t>select_one ny01y01</t>
+  </si>
+  <si>
+    <t>favorite_cover_crop</t>
+  </si>
+  <si>
+    <t>14. Do you have a favorite cover crop?</t>
+  </si>
+  <si>
+    <t>select_one xv1mj93</t>
+  </si>
+  <si>
+    <t>favorite_winter_cover_crop</t>
+  </si>
+  <si>
+    <t>14a. Which is your favorite? (winter cover crop)</t>
+  </si>
+  <si>
+    <t>${favorite_cover_crop} = 'yes'</t>
+  </si>
+  <si>
+    <t>insured_acres</t>
+  </si>
+  <si>
+    <t>15. As of today, how many of your total cropped acres are enrolled in crop insurance? [acres]</t>
+  </si>
+  <si>
+    <t>removed_insurance</t>
+  </si>
+  <si>
+    <t>16. Have you removed crop insurance on any of your fields due to cover cropping?</t>
+  </si>
+  <si>
+    <t>if_yes_remove_insurance_note</t>
+  </si>
+  <si>
+    <t>16.a  If you selected "Yes," please provide additional details.</t>
+  </si>
+  <si>
+    <t>${removed_insurance} = 'yes'</t>
+  </si>
+  <si>
+    <t>claim_cover_crop</t>
+  </si>
+  <si>
+    <t>17.  Have you ever had problems filing a crop insurance claim because of using cover crops?</t>
+  </si>
+  <si>
+    <t>if_yes_claim_note</t>
+  </si>
+  <si>
+    <t>17.a  If you selected "Yes," please provide additional details.</t>
+  </si>
+  <si>
+    <t>${claim_cover_crop} = 'yes'</t>
+  </si>
+  <si>
+    <t>tilled_acres</t>
+  </si>
+  <si>
+    <t>18. As of today, how many of your total cropped acres are tilled? [# acres, enter "0" if none]</t>
+  </si>
+  <si>
+    <t>select_one ow12s70</t>
+  </si>
+  <si>
+    <t>farm_tillage_type</t>
+  </si>
+  <si>
+    <t>18.a Clarification:  Do you consider your operation:</t>
+  </si>
+  <si>
+    <t>${tilled_acres} &gt; 0</t>
+  </si>
+  <si>
+    <t>tillage_it_depends</t>
+  </si>
+  <si>
+    <t>18. a1 Clarification: If you selected "it depends", please describe.</t>
+  </si>
+  <si>
+    <t>${farm_tillage_type} = 'depends'</t>
+  </si>
+  <si>
+    <t>previous_tillage</t>
+  </si>
+  <si>
+    <t>18.b Clarification: Have you ever tilled any of your cropped acres?</t>
+  </si>
+  <si>
+    <t>${tilled_acres} = 0</t>
+  </si>
+  <si>
+    <t>years_since_tillage</t>
+  </si>
+  <si>
+    <t>18.c Clarification:  How many years since you last tilled any of your acres? [# of years]</t>
+  </si>
+  <si>
+    <t>${previous_tillage} = 'yes' and ${tilled_acres} = 0</t>
+  </si>
+  <si>
+    <t>tilled_acres_cover_crop</t>
+  </si>
+  <si>
+    <t>19. How many of your COVER CROPPED acres are tilled? [# of acres, enter "0" if none]</t>
+  </si>
+  <si>
+    <t>tillage_type_cover_crop</t>
+  </si>
+  <si>
+    <t>19.a What kind of tillage are you doing on the COVER CROPPED acres?</t>
+  </si>
+  <si>
+    <t>${tilled_acres_cover_crop} &gt; 0</t>
+  </si>
+  <si>
+    <t>tillage_cover_crop_it_depends</t>
+  </si>
+  <si>
+    <t>19. a1 Clarification: If you selected "it depends", please describe.</t>
+  </si>
+  <si>
+    <t>${tillage_type_cover_crop} = 'depends'</t>
+  </si>
+  <si>
+    <t>previous_tillage_cover_crop</t>
+  </si>
+  <si>
+    <t>19.b Clarification: Have you ever tilled your COVER CROPPED acres?</t>
+  </si>
+  <si>
+    <t>${tilled_acres_cover_crop} = 0</t>
+  </si>
+  <si>
+    <t>years_since_tillage_cover_crop</t>
+  </si>
+  <si>
+    <t>19.c Clarification: How many years since you last tilled your COVER CROPPED acres? [# of years]</t>
+  </si>
+  <si>
+    <t>${previous_tillage_cover_crop} = 'yes' and ${tilled_acres_cover_crop} = 0</t>
+  </si>
+  <si>
+    <t>info_sources</t>
+  </si>
+  <si>
+    <t>20. What sources of information do you seek out and use to learn more about cover crops?</t>
+  </si>
+  <si>
+    <t>dst_use</t>
+  </si>
+  <si>
+    <t>21. Do you use any decision support tools. (e.g, spreadsheets, worksheets, or software tools provided by NRCS, extension specialists, or crop advisors)?</t>
+  </si>
+  <si>
+    <t>software_use</t>
+  </si>
+  <si>
+    <t>22. What types of software, if any, do you use to manage your farm data?</t>
+  </si>
+  <si>
+    <t>devices_use</t>
+  </si>
+  <si>
+    <t>23. What type of devices do you use in your agricultural operations (iPad, computer, smartphone)?</t>
+  </si>
+  <si>
+    <t>yield_monitor</t>
+  </si>
+  <si>
+    <t>24. Where do you store your yield monitor data?</t>
+  </si>
+  <si>
+    <t>yield_data_share</t>
+  </si>
+  <si>
+    <t>25. Do you feel comfortable sharing yield monitor data?</t>
+  </si>
+  <si>
+    <t>percent_rented</t>
+  </si>
+  <si>
+    <t>26. Approximately what percentage of the acres you farm are rented?</t>
+  </si>
+  <si>
+    <t>why_participating</t>
+  </si>
+  <si>
+    <t>27. Why are you participating in this study?</t>
+  </si>
+  <si>
+    <t>generalfarmendnote</t>
+  </si>
+  <si>
+    <t>You've reached the end of the general farm questions. The next section refers to just the site (or sites) with the cover crop trial. Swipe over to the next screen to continue.</t>
+  </si>
+  <si>
+    <t>begin_repeat</t>
+  </si>
+  <si>
+    <t>group_code_field_history</t>
+  </si>
+  <si>
+    <t>Group - PSA Site Specific Questions</t>
+  </si>
+  <si>
+    <t>site_specifics</t>
+  </si>
+  <si>
+    <t>The following questions pertain to the specific field(s) that your grower has in trial. If the grower has multiple fields in trial, you will be prompted to enter information about each trial separately.</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>1. Please enter the trial code [3-letter code]</t>
+  </si>
+  <si>
+    <t>select_one ql6ce98</t>
+  </si>
+  <si>
+    <t>years_cover_crop</t>
+  </si>
+  <si>
+    <t>2. How long has this site been cover cropped?</t>
+  </si>
+  <si>
+    <t>insured</t>
+  </si>
+  <si>
+    <t>3. Is the trial field enrolled in crop insurance?</t>
+  </si>
+  <si>
+    <t>select_one ab12c34</t>
+  </si>
+  <si>
+    <t>rent_own</t>
+  </si>
+  <si>
+    <t>4. Is the trial field on rented or owned land?</t>
+  </si>
+  <si>
+    <t>code_crop_rotation</t>
+  </si>
+  <si>
+    <t>5. What cash crops are GENERALLY in your crop rotation for this field?</t>
+  </si>
+  <si>
+    <t>select_one dq65c45</t>
+  </si>
+  <si>
+    <t>previous_crop</t>
+  </si>
+  <si>
+    <t>6. What was the previous crop last year in this field?</t>
+  </si>
+  <si>
+    <t>select_one sv07f73</t>
+  </si>
+  <si>
+    <t>previous_fert</t>
+  </si>
+  <si>
+    <t>7. How much total Nitrogen fertility was applied to the previous crop (approximately)? [lbs]</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>cover_crop_plant_date</t>
+  </si>
+  <si>
+    <t>8. When was the COVER CROP planted?</t>
+  </si>
+  <si>
+    <t>If an exact date is not known, please enter approximately, to the closest week or month.</t>
+  </si>
+  <si>
+    <t>select_one ji9wb83</t>
+  </si>
+  <si>
+    <t>cover_crop_planting_method</t>
+  </si>
+  <si>
+    <t>9. How was the cover crop planted?</t>
+  </si>
+  <si>
+    <t>select_multiple xv1mj93</t>
+  </si>
+  <si>
+    <t>cover_crop_spp</t>
+  </si>
+  <si>
+    <t>10. What cover crop species are planted?</t>
+  </si>
+  <si>
+    <t>cover_crop_rate_total</t>
+  </si>
+  <si>
+    <t>11. What is the approximate total rate of all cover crop planted? (in lbs/ acre)</t>
+  </si>
+  <si>
+    <t>cover_crop_litter</t>
+  </si>
+  <si>
+    <t>12. Do you apply litter or fertility to your cover crop?</t>
+  </si>
+  <si>
+    <t>cover_crop_tillage</t>
+  </si>
+  <si>
+    <t>13. Do you do any tillage prior to terminating the COVER crop? (ie: subsoiling)</t>
+  </si>
+  <si>
+    <t>cover_crop_tillage_type</t>
+  </si>
+  <si>
+    <t>13 a. If Yes, please describe?</t>
+  </si>
+  <si>
+    <t>${cover_crop_tillage} = 'yes'</t>
+  </si>
+  <si>
+    <t>select_one cl4gf13</t>
+  </si>
+  <si>
+    <t>cover_crop_termination</t>
+  </si>
+  <si>
+    <t>14. How do you terminate your COVER crop?</t>
+  </si>
+  <si>
+    <t>select_multiple bd5he26</t>
+  </si>
+  <si>
+    <t>cover_crop_termination_herbicide</t>
+  </si>
+  <si>
+    <t>15. What herbicides do you plan to use?</t>
+  </si>
+  <si>
+    <t>select_one bg45t67</t>
+  </si>
+  <si>
+    <t>crop</t>
+  </si>
+  <si>
+    <t>16. What is/ will be this year's crop?</t>
+  </si>
+  <si>
+    <t>(*reminder* to participate in this trial, fields can only be planted in corn, soybean, or cotton)</t>
+  </si>
+  <si>
+    <t>crop_variety</t>
+  </si>
+  <si>
+    <t>17. What is the variety of the crop?</t>
+  </si>
+  <si>
+    <t>crop_maturity</t>
+  </si>
+  <si>
+    <t>18. What is the maturity of the crop? (ie, number of days to harvest or soybean maturity group, or other)</t>
+  </si>
+  <si>
+    <t>crop_tillage</t>
+  </si>
+  <si>
+    <t>19. Will you do any type of tillage on this crop?</t>
+  </si>
+  <si>
+    <t>Technicians: this trial uses only fields with conservation tillage practices, in which the surface residue of a cover crop remains intact. However some growers choose to preform some form of tillage, like strip tilling, or vertical tillage. It is important to record any soil disturbance for the water infiltration modeling team.</t>
+  </si>
+  <si>
+    <t>crop_tillage_type</t>
+  </si>
+  <si>
+    <t>19 a. If yes, please describe tillage.</t>
+  </si>
+  <si>
+    <t>${crop_tillage} = 'yes'</t>
+  </si>
+  <si>
+    <t>crop_fert</t>
+  </si>
+  <si>
+    <t>20. How much total Nitrogen fertilizer will this year's crop receive?</t>
+  </si>
+  <si>
+    <t>more_farm_info</t>
+  </si>
+  <si>
+    <t>21. Are there other considerations or things you want us to know about this field? (why you plant cover crops there, it stays very wet, it's generally high biomass, it's new to cover crops, etc.)</t>
+  </si>
+  <si>
+    <t>notegroupselect</t>
+  </si>
+  <si>
+    <t>If this farm has more than 1 site/ trial for this grower, click the plus icon to add an additional site. A new group of questions will appear on the screen, above the +, so you will have to scroll back up.</t>
+  </si>
+  <si>
+    <t>end_repeat</t>
+  </si>
+  <si>
+    <t>note_end</t>
+  </si>
+  <si>
+    <t>Thank you for completing the Survey. Swipe to the next screen for a Timeline to share with your grower. Continue swiping until you reach the end to Submit.</t>
+  </si>
+  <si>
+    <t>note_to_farmer</t>
+  </si>
+  <si>
+    <t>A Timeline to share with your grower: a technician will be in contact this spring. Cover Crop biomass is collected in the spring at the time it is terminated.  For our saftey it is nice to harvest biomass right before burndown. Please notify the technician when you think you will terminate, and we can harvest +/- 3 to 4 days around that time. We can also return following herbicide application, when safe to do so. We will return when the crop is planted.  When do you think that will be? How long after terminating the cover crop? It is important to record those dates. We will install moisture sensors in between the crop rows after it has emerged.  Please do all of your fertilizer applications, and other management operations the same as you always would in that field. Our equipment is designed to be sprayed over.  We will raise a solar panel after the crop has closed canopy. We will come take yield data by hand in a 10 foot section around the soil moisture sensors before you harvest with your combine. Please notify us when you will: terminate your cover crop, after crop planting, and before harvest.  Thank you.</t>
+  </si>
+  <si>
+    <t>note_to_tech</t>
+  </si>
+  <si>
+    <t>Technician: If there are questions that you were unable to complete at this time, you may save the survey to your device to retrieve later by clicking the arrow with the dot, selecting 'Go to End', naming the form by the farm name,  and select "Save Form and Exit". Forms can be retrieved in your "Saved Forms"</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yy77y77</t>
+  </si>
+  <si>
+    <t>farm</t>
+  </si>
+  <si>
     <t>Farm</t>
   </si>
   <si>
-    <t>group_social_sci_survey</t>
-  </si>
-  <si>
-    <t>General Whole Farm Survey</t>
-  </si>
-  <si>
-    <t>note5</t>
-  </si>
-  <si>
-    <t>Please have the grower respond to the questions that follow.</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>crop_acres</t>
-  </si>
-  <si>
-    <t>8. As of today, how many total acres do you plant in crops? [acres]</t>
-  </si>
-  <si>
-    <t>select_multiple dq65c45</t>
-  </si>
-  <si>
-    <t>farm_crop_rotation</t>
-  </si>
-  <si>
-    <t>9. What crops are GENERALLY in your crop rotation?</t>
-  </si>
-  <si>
-    <t>cover_crop_acres</t>
-  </si>
-  <si>
-    <t>10. As of today, how many of your total cropped acres are in COVER CROPS? [acres]</t>
-  </si>
-  <si>
-    <t>cover_crop_acres_terminated</t>
-  </si>
-  <si>
-    <t>10.a Clarification:  If COVER CROPS have already been terminated, how many acres did you have of winter cover crops prior to termination? [# acres, or leave blank if not applicable]</t>
-  </si>
-  <si>
-    <t>${cover_crop_acres} = 0</t>
-  </si>
-  <si>
-    <t>cover_crop_acres_typical</t>
-  </si>
-  <si>
-    <t>11.  If this was a particularly bad or otherwise non-representative year, how many acres do you typically have of winter COVER CROPS?  [# acres, or leave blank if not applicable]</t>
-  </si>
-  <si>
-    <t>first_year_cover_crop</t>
-  </si>
-  <si>
-    <t>12. In what year did you first plant COVER CROPS? [four digit year, example : 1985] *reminder, for a grower to participate, this may not be their first time planting cover crops</t>
-  </si>
-  <si>
-    <t>select_one xe2wp37</t>
-  </si>
-  <si>
-    <t>every_year</t>
-  </si>
-  <si>
-    <t>13. Have you planted COVER CROPS every year since?</t>
-  </si>
-  <si>
-    <t>favorite_cover_crop</t>
-  </si>
-  <si>
-    <t>14. Do you have a favorite cover crop?</t>
-  </si>
-  <si>
-    <t>select_one xv1mj93</t>
-  </si>
-  <si>
-    <t>favorite_winter_cover_crop</t>
-  </si>
-  <si>
-    <t>14a. Which is your favorite? (winter cover crop)</t>
-  </si>
-  <si>
-    <t>${favorite_cover_crop} = 'yes'</t>
-  </si>
-  <si>
-    <t>insured_acres</t>
-  </si>
-  <si>
-    <t>15. As of today, how many of your total cropped acres are enrolled in crop insurance? [acres]</t>
-  </si>
-  <si>
-    <t>removed_insurance</t>
-  </si>
-  <si>
-    <t>16. Have you removed crop insurance on any of your fields due to cover cropping?</t>
-  </si>
-  <si>
-    <t>if_yes_remove_insurance_note</t>
-  </si>
-  <si>
-    <t>16.a  If you selected "Yes," please provide additional details.</t>
-  </si>
-  <si>
-    <t>${removed_insurance} = 'yes'</t>
-  </si>
-  <si>
-    <t>claim_cover_crop</t>
-  </si>
-  <si>
-    <t>17.  Have you ever had problems filing a crop insurance claim because of using cover crops?</t>
-  </si>
-  <si>
-    <t>if_yes_claim_note</t>
-  </si>
-  <si>
-    <t>17.a  If you selected "Yes," please provide additional details.</t>
-  </si>
-  <si>
-    <t>${claim_cover_crop} = 'yes'</t>
-  </si>
-  <si>
-    <t>tilled_acres</t>
-  </si>
-  <si>
-    <t>18. As of today, how many of your total cropped acres are tilled? [# acres, enter "0" if none]</t>
-  </si>
-  <si>
-    <t>${tilled_acres} &gt; 0</t>
-  </si>
-  <si>
-    <t>18. a1 Clarification: If you selected "it depends", please describe.</t>
-  </si>
-  <si>
-    <t>previous_tillage</t>
-  </si>
-  <si>
-    <t>18.b Clarification: Have you ever tilled any of your cropped acres?</t>
-  </si>
-  <si>
-    <t>${tilled_acres} = 0</t>
-  </si>
-  <si>
-    <t>years_since_tillage</t>
-  </si>
-  <si>
-    <t>18.c Clarification:  How many years since you last tilled any of your acres? [# of years]</t>
-  </si>
-  <si>
-    <t>${previous_tillage} = 'yes' and ${tilled_acres} = 0</t>
-  </si>
-  <si>
-    <t>tilled_acres_cover_crop</t>
-  </si>
-  <si>
-    <t>19. How many of your COVER CROPPED acres are tilled? [# of acres, enter "0" if none]</t>
-  </si>
-  <si>
-    <t>tillage_type_cover_crop</t>
-  </si>
-  <si>
-    <t>${tilled_acres_cover_crop} &gt; 0</t>
-  </si>
-  <si>
-    <t>previous_tillage_cover_crop</t>
-  </si>
-  <si>
-    <t>19.b Clarification: Have you ever tilled your COVER CROPPED acres?</t>
-  </si>
-  <si>
-    <t>${tilled_acres_cover_crop} = 0</t>
-  </si>
-  <si>
-    <t>years_since_tillage_cover_crop</t>
-  </si>
-  <si>
-    <t>19.c Clarification: How many years since you last tilled your COVER CROPPED acres? [# of years]</t>
-  </si>
-  <si>
-    <t>${previous_tillage_cover_crop} = 'yes' and ${tilled_acres_cover_crop} = 0</t>
-  </si>
-  <si>
-    <t>info_sources</t>
-  </si>
-  <si>
-    <t>20. What sources of information do you seek out and use to learn more about cover crops?</t>
-  </si>
-  <si>
-    <t>dst_use</t>
-  </si>
-  <si>
-    <t>21. Do you use any decision support tools. (e.g, spreadsheets, worksheets, or software tools provided by NRCS, extension specialists, or crop advisors)?</t>
-  </si>
-  <si>
-    <t>software_use</t>
-  </si>
-  <si>
-    <t>22. What types of software, if any, do you use to manage your farm data?</t>
-  </si>
-  <si>
-    <t>devices_use</t>
-  </si>
-  <si>
-    <t>23. What type of devices do you use in your agricultural operations (iPad, computer, smartphone)?</t>
-  </si>
-  <si>
-    <t>yield_monitor</t>
-  </si>
-  <si>
-    <t>24. Where do you store your yield monitor data?</t>
-  </si>
-  <si>
-    <t>yield_data_share</t>
-  </si>
-  <si>
-    <t>25. Do you feel comfortable sharing yield monitor data?</t>
-  </si>
-  <si>
-    <t>percent_rented</t>
-  </si>
-  <si>
-    <t>26. Approximately what percentage of the acres you farm are rented?</t>
-  </si>
-  <si>
-    <t>why_participating</t>
-  </si>
-  <si>
-    <t>27. Why are you participating in this study?</t>
-  </si>
-  <si>
-    <t>You've reached the end of the general farm questions. The next section refers to just the site (or sites) with the cover crop trial. Swipe over to the next screen to continue.</t>
-  </si>
-  <si>
-    <t>begin_repeat</t>
-  </si>
-  <si>
-    <t>group_code_field_history</t>
-  </si>
-  <si>
-    <t>Group - PSA Site Specific Questions</t>
-  </si>
-  <si>
-    <t>site_specifics</t>
-  </si>
-  <si>
-    <t>The following questions pertain to the specific field(s) that your grower has in trial. If the grower has multiple fields in trial, you will be prompted to enter information about each trial separately.</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>1. Please enter the trial code [3-letter code]</t>
-  </si>
-  <si>
-    <t>select_one ql6ce98</t>
-  </si>
-  <si>
-    <t>years_cover_crop</t>
-  </si>
-  <si>
-    <t>2. How long has this site been cover cropped?</t>
-  </si>
-  <si>
-    <t>insured</t>
-  </si>
-  <si>
-    <t>3. Is the trial field enrolled in crop insurance?</t>
-  </si>
-  <si>
-    <t>select_one ab12c34</t>
-  </si>
-  <si>
-    <t>rent_own</t>
-  </si>
-  <si>
-    <t>4. Is the trial field on rented or owned land?</t>
-  </si>
-  <si>
-    <t>code_crop_rotation</t>
-  </si>
-  <si>
-    <t>5. What cash crops are GENERALLY in your crop rotation for this field?</t>
-  </si>
-  <si>
-    <t>select_one dq65c45</t>
-  </si>
-  <si>
-    <t>previous_crop</t>
-  </si>
-  <si>
-    <t>6. What was the previous crop last year in this field?</t>
-  </si>
-  <si>
-    <t>select_one sv07f73</t>
-  </si>
-  <si>
-    <t>previous_fert</t>
-  </si>
-  <si>
-    <t>7. How much total Nitrogen fertility was applied to the previous crop (approximately)? [lbs]</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>cover_crop_plant_date</t>
-  </si>
-  <si>
-    <t>8. When was the COVER CROP planted?</t>
-  </si>
-  <si>
-    <t>If an exact date is not known, please enter approximately, to the closest week or month.</t>
-  </si>
-  <si>
-    <t>select_one ji9wb83</t>
-  </si>
-  <si>
-    <t>cover_crop_planting_method</t>
-  </si>
-  <si>
-    <t>9. How was the cover crop planted?</t>
-  </si>
-  <si>
-    <t>select_multiple xv1mj93</t>
-  </si>
-  <si>
-    <t>cover_crop_spp</t>
-  </si>
-  <si>
-    <t>10. What cover crop species are planted?</t>
-  </si>
-  <si>
-    <t>cover_crop_rate_total</t>
-  </si>
-  <si>
-    <t>11. What is the approximate total rate of all cover crop planted? (in lbs/ acre)</t>
-  </si>
-  <si>
-    <t>cover_crop_litter</t>
-  </si>
-  <si>
-    <t>12. Do you apply litter or fertility to your cover crop?</t>
-  </si>
-  <si>
-    <t>cover_crop_tillage</t>
-  </si>
-  <si>
-    <t>13. Do you do any tillage prior to terminating the COVER crop? (ie: subsoiling)</t>
-  </si>
-  <si>
-    <t>cover_crop_tillage_type</t>
-  </si>
-  <si>
-    <t>13 a. If Yes, please describe?</t>
-  </si>
-  <si>
-    <t>${cover_crop_tillage} = 'yes'</t>
-  </si>
-  <si>
-    <t>select_one cl4gf13</t>
-  </si>
-  <si>
-    <t>cover_crop_termination</t>
-  </si>
-  <si>
-    <t>14. How do you terminate your COVER crop?</t>
-  </si>
-  <si>
-    <t>select_multiple bd5he26</t>
-  </si>
-  <si>
-    <t>cover_crop_termination_herbicide</t>
-  </si>
-  <si>
-    <t>15. What herbicides do you plan to use?</t>
-  </si>
-  <si>
-    <t>select_one bg45t67</t>
-  </si>
-  <si>
-    <t>crop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16. What is/ will be this year's crop? </t>
-  </si>
-  <si>
-    <t>(*reminder* to participate in this trial, fields can only be planted in corn, soybean, or cotton)</t>
-  </si>
-  <si>
-    <t>crop_variety</t>
-  </si>
-  <si>
-    <t>17. What is the variety of the crop?</t>
-  </si>
-  <si>
-    <t>crop_maturity</t>
-  </si>
-  <si>
-    <t>18. What is the maturity of the crop? (ie, number of days to harvest or soybean maturity group, or other)</t>
-  </si>
-  <si>
-    <t>crop_tillage</t>
-  </si>
-  <si>
-    <t>19. Will you do any type of tillage on this crop?</t>
-  </si>
-  <si>
-    <t>Technicians: this trial uses only fields with conservation tillage practices, in which the surface residue of a cover crop remains intact. However some growers choose to preform some form of tillage, like minimal strip tilling, subsoiling at a 45 degree angle, or vertical tillage. It is important to record any soil disturbance for the water infiltration modeling team.</t>
-  </si>
-  <si>
-    <t>crop_tillage_type</t>
-  </si>
-  <si>
-    <t>19 a. If yes, please describe tillage.</t>
-  </si>
-  <si>
-    <t>${crop_tillage} = 'yes'</t>
-  </si>
-  <si>
-    <t>crop_fert</t>
-  </si>
-  <si>
-    <t>20. How much total Nitrogen fertilizer will this year's crop receive?</t>
-  </si>
-  <si>
-    <t>more_farm_info</t>
-  </si>
-  <si>
-    <t>21. Are there other considerations or things you want us to know about this field? (why you plant cover crops there, it stays very wet, it's generally high biomass, it's new to cover crops, etc.)</t>
-  </si>
-  <si>
-    <t>notegroupselect</t>
-  </si>
-  <si>
-    <t>If this farm has more than 1 site/ trial for this grower, click the plus icon to add an additional site. A new group of questions will appear on the screen, above the +, so you will have to scroll back up.</t>
-  </si>
-  <si>
-    <t>end_repeat</t>
-  </si>
-  <si>
-    <t>note_end</t>
-  </si>
-  <si>
-    <t>Thank you for completing the Survey. Swipe to the next screen for a Timeline to share with your grower. Continue swiping until you reach the end to Submit.</t>
-  </si>
-  <si>
-    <t>note_to_farmer</t>
-  </si>
-  <si>
-    <t>A Timeline to share with your grower: a technician will be in contact this spring. Cover Crop biomass is collected in the spring at the time it is terminated.  For our saftey it is nice to harvest biomass right before burndown. Please notify the technician when you think you will terminate, and we can harvest +/- 3 to 4 days around that time. We can also return following herbicide application, when safe to do so. We will return when the crop is planted.  When do you think that will be? How long after terminating the cover crop? It is important to record those dates. We will install moisture sensors in between the crop rows after it has emerged.  Please do all of your fertilizer applications, and other management operations the same as you always would in that field. Our equipment is designed to be sprayed over.  We will raise a solar panel after the crop has closed canopy. We will come take yield data by hand in a 10 foot section around the soil moisture sensors before you harvest with your combine. Please notify us when you will: terminate your cover crop, after crop planting, and before harvest.  Thank you.</t>
-  </si>
-  <si>
-    <t>note_to_tech</t>
-  </si>
-  <si>
-    <t>Technician: If there are questions that you were unable to complete at this time, you may save the survey to your device to retrieve later by clicking the arrow with the dot, selecting 'Go to End', naming the form by the farm name,  and select "Save Form and Exit". Forms can be retrieved in your "Saved Forms"</t>
-  </si>
-  <si>
-    <t>list_name</t>
-  </si>
-  <si>
-    <t>yy77y77</t>
-  </si>
-  <si>
-    <t>farm</t>
-  </si>
-  <si>
     <t>research_station</t>
   </si>
   <si>
@@ -761,6 +803,9 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>ny01y01</t>
+  </si>
+  <si>
     <t>no</t>
   </si>
   <si>
@@ -1149,51 +1194,6 @@
   </si>
   <si>
     <t>bg45t67</t>
-  </si>
-  <si>
-    <t>noteswipe</t>
-  </si>
-  <si>
-    <t>farm_or_station</t>
-  </si>
-  <si>
-    <t>${farm_or_station} = 'farm'</t>
-  </si>
-  <si>
-    <t>generalfarmendnote</t>
-  </si>
-  <si>
-    <t>select_one ow12s70</t>
-  </si>
-  <si>
-    <t>18.a Clarification:  Do you consider your operation:</t>
-  </si>
-  <si>
-    <t>farm_tillage_type</t>
-  </si>
-  <si>
-    <t>selected(${farm_tillage_type}, 'depends')</t>
-  </si>
-  <si>
-    <t>tillage_it_depends</t>
-  </si>
-  <si>
-    <t>19.a What kind of tillage are you doing on the COVER CROPPED acres?</t>
-  </si>
-  <si>
-    <t>19. a1 Clarification: If you selected "it depends", please describe.</t>
-  </si>
-  <si>
-    <t>tillage_cover_crop_it_depends</t>
-  </si>
-  <si>
-    <t>selected(${tillage_cover_crop_it_depends}, 'depends')</t>
-  </si>
-  <si>
-    <t>ny01y01</t>
-  </si>
-  <si>
-    <t>select_one ny01y01</t>
   </si>
 </sst>
 </file>
@@ -1209,30 +1209,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1247,12 +1229,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1559,15 +1537,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90:XFD90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="46.36328125" customWidth="1"/>
+    <col min="1" max="1" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.08984375" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -1740,10 +1718,10 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>376</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
@@ -1754,10 +1732,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
@@ -1768,13 +1746,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
@@ -1782,7 +1760,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>40</v>
@@ -1796,7 +1774,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>42</v>
@@ -1810,7 +1788,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
         <v>44</v>
@@ -1824,7 +1802,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
         <v>46</v>
@@ -1833,18 +1811,18 @@
         <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
@@ -1852,13 +1830,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
         <v>15</v>
@@ -1871,16 +1849,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>377</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1888,10 +1866,10 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
@@ -1900,7 +1878,7 @@
         <v>16</v>
       </c>
       <c r="H24" t="s">
-        <v>378</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1908,10 +1886,10 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -1919,13 +1897,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
         <v>15</v>
@@ -1933,13 +1911,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E27" t="s">
         <v>15</v>
@@ -1947,13 +1925,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
@@ -1961,30 +1939,30 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
       </c>
       <c r="H29" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1992,27 +1970,27 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
-        <v>74</v>
+      <c r="A32" t="s">
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
@@ -2020,13 +1998,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>390</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
@@ -2034,30 +2012,30 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
       </c>
       <c r="H34" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
@@ -2065,13 +2043,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>390</v>
+        <v>79</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E36" t="s">
         <v>15</v>
@@ -2079,30 +2057,30 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C37" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E37" t="s">
         <v>15</v>
       </c>
       <c r="H37" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>390</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
@@ -2110,194 +2088,194 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
       </c>
       <c r="H39" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B40" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+      <c r="C40" t="s">
+        <v>99</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
-        <v>380</v>
+      <c r="A41" t="s">
+        <v>100</v>
       </c>
       <c r="B41" t="s">
-        <v>382</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>381</v>
+        <v>101</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
       </c>
       <c r="H41" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>98</v>
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" t="s">
+        <v>105</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>383</v>
+      <c r="H42" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
-        <v>390</v>
+      <c r="A43" t="s">
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
-      </c>
-      <c r="C43" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" t="s">
+        <v>108</v>
+      </c>
+      <c r="E43" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" t="s">
+        <v>111</v>
+      </c>
+      <c r="E44" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>100</v>
       </c>
-      <c r="E43" t="s">
-        <v>15</v>
-      </c>
-      <c r="H43" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44" t="s">
-        <v>102</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H44" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" s="4" t="s">
-        <v>380</v>
-      </c>
       <c r="B46" t="s">
-        <v>107</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>385</v>
+        <v>115</v>
+      </c>
+      <c r="C46" t="s">
+        <v>116</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
       </c>
       <c r="H46" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>386</v>
+      <c r="A47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" t="s">
+        <v>119</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
       </c>
-      <c r="H47" s="1" t="s">
-        <v>388</v>
+      <c r="H47" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="4" t="s">
-        <v>390</v>
+      <c r="A48" t="s">
+        <v>79</v>
       </c>
       <c r="B48" t="s">
-        <v>109</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>110</v>
+        <v>121</v>
+      </c>
+      <c r="C48" t="s">
+        <v>122</v>
       </c>
       <c r="E48" t="s">
         <v>15</v>
       </c>
       <c r="H48" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>112</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
+      </c>
+      <c r="C49" t="s">
+        <v>125</v>
       </c>
       <c r="E49" t="s">
         <v>15</v>
       </c>
       <c r="H49" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="C50" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="E50" t="s">
         <v>15</v>
@@ -2305,13 +2283,13 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="C51" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="E51" t="s">
         <v>15</v>
@@ -2319,13 +2297,13 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="C52" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="E52" t="s">
         <v>15</v>
@@ -2333,13 +2311,13 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B53" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="C53" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>
@@ -2347,13 +2325,13 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B54" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="C54" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="E54" t="s">
         <v>15</v>
@@ -2361,13 +2339,13 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>390</v>
+        <v>79</v>
       </c>
       <c r="B55" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C55" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="E55" t="s">
         <v>15</v>
@@ -2375,13 +2353,13 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B56" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="C56" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="E56" t="s">
         <v>15</v>
@@ -2389,13 +2367,13 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B57" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C57" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="E57" t="s">
         <v>15</v>
@@ -2406,10 +2384,10 @@
         <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>379</v>
+        <v>143</v>
       </c>
       <c r="C58" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="E58" t="s">
         <v>15</v>
@@ -2422,13 +2400,13 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="B60" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="C60" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
@@ -2442,10 +2420,10 @@
         <v>17</v>
       </c>
       <c r="B61" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C61" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="E61" t="s">
         <v>15</v>
@@ -2453,41 +2431,41 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B62" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="C62" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="E62" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="B63" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="C63" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="E63" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="C64" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="E64" t="s">
         <v>15</v>
@@ -2495,13 +2473,13 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="B65" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="C65" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="E65" t="s">
         <v>15</v>
@@ -2509,13 +2487,13 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="C66" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="E66" t="s">
         <v>15</v>
@@ -2523,27 +2501,27 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B67" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C67" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="E67" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="B68" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="C68" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="E68" t="s">
         <v>15</v>
@@ -2551,30 +2529,30 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="B69" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="C69" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="D69" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="E69" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="B70" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="C70" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -2582,13 +2560,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B71" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="C71" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="E71" t="s">
         <v>15</v>
@@ -2596,13 +2574,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B72" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="C72" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="E72" t="s">
         <v>15</v>
@@ -2610,13 +2588,13 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>390</v>
+        <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="C73" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="E73" t="s">
         <v>15</v>
@@ -2624,44 +2602,44 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>390</v>
+        <v>79</v>
       </c>
       <c r="B74" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="C74" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="E74" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B75" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C75" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="E75" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="H75" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="B76" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="C76" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="E76" t="s">
         <v>15</v>
@@ -2669,13 +2647,13 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="B77" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="C77" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="E77" t="s">
         <v>15</v>
@@ -2683,16 +2661,16 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="B78" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="C78" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="D78" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="E78" t="s">
         <v>15</v>
@@ -2700,13 +2678,13 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B79" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="C79" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="E79" t="s">
         <v>15</v>
@@ -2714,13 +2692,13 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B80" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="C80" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="E80" t="s">
         <v>15</v>
@@ -2728,47 +2706,47 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>390</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="C81" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="D81" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="E81" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B82" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="C82" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="E82" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H82" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="B83" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="C83" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
@@ -2776,13 +2754,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B84" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="C84" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="E84" t="s">
         <v>15</v>
@@ -2793,10 +2771,10 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="C85" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="E85" t="s">
         <v>15</v>
@@ -2804,7 +2782,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
@@ -2812,10 +2790,10 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="C87" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
@@ -2826,10 +2804,10 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="C88" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
@@ -2840,10 +2818,10 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="C89" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="E89" t="s">
         <v>15</v>
@@ -2858,18 +2836,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="22" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2880,959 +2853,959 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="C5" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="C7" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="C8" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B9" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="C9" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B10" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="C10" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B11" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="C11" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B12" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="C12" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="C13" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B14" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="C14" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B15" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="C15" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B16" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="C16" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B17" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="C17" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>243</v>
+      <c r="A18" t="s">
+        <v>255</v>
+      </c>
+      <c r="B18" t="s">
+        <v>256</v>
+      </c>
+      <c r="C18" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>245</v>
+      <c r="A19" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" t="s">
+        <v>258</v>
+      </c>
+      <c r="C19" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>389</v>
+        <v>260</v>
       </c>
       <c r="B20" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="C20" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>389</v>
+        <v>260</v>
       </c>
       <c r="B21" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="C21" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B22" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="C22" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B23" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
       <c r="C23" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B24" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="C24" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B25" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="C25" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B26" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="C26" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B27" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="C27" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B28" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="C28" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B29" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="C29" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B30" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="C30" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B31" t="s">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="C31" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B32" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="C32" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B33" t="s">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="C33" t="s">
-        <v>270</v>
+        <v>285</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B34" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="C34" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B35" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="C35" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B36" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="C36" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B37" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c r="C37" t="s">
-        <v>278</v>
+        <v>293</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B38" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="C38" t="s">
-        <v>280</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B39" t="s">
-        <v>281</v>
+        <v>296</v>
       </c>
       <c r="C39" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B40" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="C40" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B41" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="C41" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>291</v>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>300</v>
+      </c>
+      <c r="B42" t="s">
+        <v>301</v>
+      </c>
+      <c r="C42" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>300</v>
+      </c>
+      <c r="B43" t="s">
+        <v>303</v>
+      </c>
+      <c r="C43" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>300</v>
+      </c>
+      <c r="B44" t="s">
+        <v>305</v>
+      </c>
+      <c r="C44" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="B45" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="C45" t="s">
-        <v>294</v>
+        <v>309</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="B46" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="C46" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="B47" t="s">
-        <v>297</v>
+        <v>312</v>
       </c>
       <c r="C47" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="B48" t="s">
-        <v>299</v>
+        <v>314</v>
       </c>
       <c r="C48" t="s">
-        <v>300</v>
+        <v>315</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="B49" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="C49" t="s">
-        <v>302</v>
+        <v>317</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="B50" t="s">
-        <v>303</v>
+        <v>318</v>
       </c>
       <c r="C50" t="s">
-        <v>304</v>
+        <v>319</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="B51" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="C51" t="s">
-        <v>306</v>
+        <v>321</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="B52" t="s">
-        <v>307</v>
+        <v>322</v>
       </c>
       <c r="C52" t="s">
-        <v>308</v>
+        <v>323</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>309</v>
+        <v>324</v>
       </c>
       <c r="B53" t="s">
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="C53" t="s">
-        <v>311</v>
+        <v>326</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>309</v>
+        <v>324</v>
       </c>
       <c r="B54" t="s">
-        <v>312</v>
+        <v>327</v>
       </c>
       <c r="C54" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="B55" t="s">
-        <v>315</v>
+        <v>330</v>
       </c>
       <c r="C55" t="s">
-        <v>315</v>
+        <v>330</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="B56" t="s">
-        <v>316</v>
+        <v>331</v>
       </c>
       <c r="C56" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="B57" t="s">
-        <v>318</v>
+        <v>333</v>
       </c>
       <c r="C57" t="s">
-        <v>319</v>
+        <v>334</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="B58" t="s">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="C58" t="s">
-        <v>321</v>
+        <v>336</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="B59" t="s">
-        <v>322</v>
+        <v>337</v>
       </c>
       <c r="C59" t="s">
-        <v>323</v>
+        <v>338</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="B60" t="s">
-        <v>324</v>
+        <v>339</v>
       </c>
       <c r="C60" t="s">
-        <v>325</v>
+        <v>340</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="B61" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="C61" t="s">
-        <v>327</v>
+        <v>342</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="B62" t="s">
-        <v>328</v>
+        <v>343</v>
       </c>
       <c r="C62" t="s">
-        <v>329</v>
+        <v>344</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="B63" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
       <c r="C63" t="s">
-        <v>332</v>
+        <v>347</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="B64" t="s">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="C64" t="s">
-        <v>334</v>
+        <v>349</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="B65" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="C65" t="s">
-        <v>336</v>
+        <v>351</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="B66" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="C66" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
       <c r="B67" t="s">
-        <v>338</v>
+        <v>353</v>
       </c>
       <c r="C67" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
       <c r="B68" t="s">
-        <v>340</v>
+        <v>355</v>
       </c>
       <c r="C68" t="s">
-        <v>341</v>
+        <v>356</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
       <c r="B69" t="s">
-        <v>342</v>
+        <v>357</v>
       </c>
       <c r="C69" t="s">
-        <v>343</v>
+        <v>358</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B70" t="s">
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="C70" t="s">
-        <v>346</v>
+        <v>361</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B71" t="s">
-        <v>347</v>
+        <v>362</v>
       </c>
       <c r="C71" t="s">
-        <v>348</v>
+        <v>363</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B72" t="s">
-        <v>349</v>
+        <v>364</v>
       </c>
       <c r="C72" t="s">
-        <v>350</v>
+        <v>365</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B73" t="s">
-        <v>351</v>
+        <v>366</v>
       </c>
       <c r="C73" t="s">
-        <v>352</v>
+        <v>367</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B74" t="s">
-        <v>353</v>
+        <v>368</v>
       </c>
       <c r="C74" t="s">
-        <v>354</v>
+        <v>369</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B75" t="s">
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="C75" t="s">
-        <v>356</v>
+        <v>371</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B76" t="s">
-        <v>357</v>
+        <v>372</v>
       </c>
       <c r="C76" t="s">
-        <v>358</v>
+        <v>373</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B77" t="s">
-        <v>359</v>
+        <v>374</v>
       </c>
       <c r="C77" t="s">
-        <v>360</v>
+        <v>375</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B78" t="s">
-        <v>361</v>
+        <v>376</v>
       </c>
       <c r="C78" t="s">
-        <v>362</v>
+        <v>377</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B79" t="s">
-        <v>363</v>
+        <v>378</v>
       </c>
       <c r="C79" t="s">
-        <v>364</v>
+        <v>379</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B80" t="s">
-        <v>365</v>
+        <v>380</v>
       </c>
       <c r="C80" t="s">
-        <v>366</v>
+        <v>381</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B81" t="s">
-        <v>367</v>
+        <v>382</v>
       </c>
       <c r="C81" t="s">
-        <v>368</v>
+        <v>383</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B82" t="s">
-        <v>369</v>
+        <v>384</v>
       </c>
       <c r="C82" t="s">
-        <v>370</v>
+        <v>385</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B83" t="s">
-        <v>371</v>
+        <v>386</v>
       </c>
       <c r="C83" t="s">
-        <v>372</v>
+        <v>387</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B84" t="s">
-        <v>373</v>
+        <v>388</v>
       </c>
       <c r="C84" t="s">
-        <v>374</v>
+        <v>389</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="B85" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="C85" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>375</v>
+        <v>390</v>
       </c>
       <c r="B86" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="C86" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>375</v>
+        <v>390</v>
       </c>
       <c r="B87" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="C87" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>375</v>
+        <v>390</v>
       </c>
       <c r="B88" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="C88" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3845,7 +3818,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated the psa_farm_interview form
based on feedback from the on-farm meeting, I added a few more choices to tables like: cover crops, crops, and fertility
</commit_message>
<xml_diff>
--- a/forms/psa_farm_interview/psa_farm_interview.xlsx
+++ b/forms/psa_farm_interview/psa_farm_interview.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="448">
   <si>
     <t>type</t>
   </si>
@@ -245,9 +245,6 @@
     <t>every_year</t>
   </si>
   <si>
-    <t>13. Have you planted COVER CROPS every year since?</t>
-  </si>
-  <si>
     <t>select_one ny01y01</t>
   </si>
   <si>
@@ -488,9 +485,6 @@
     <t>previous_crop</t>
   </si>
   <si>
-    <t>select_one sv07f73</t>
-  </si>
-  <si>
     <t>previous_fert</t>
   </si>
   <si>
@@ -1175,9 +1169,6 @@
     <t>30. Is the trial field on rented or owned land?</t>
   </si>
   <si>
-    <t>31. What cash crops are GENERALLY in your crop rotation for this field?</t>
-  </si>
-  <si>
     <t>32. What was the previous crop last year in this field?</t>
   </si>
   <si>
@@ -1274,9 +1265,6 @@
     <t>econ_total_cover_acres</t>
   </si>
   <si>
-    <t>39. Do you apply litter or fertility to your cover crop?</t>
-  </si>
-  <si>
     <t>40. Do you do any tillage prior to terminating the COVER crop? (ie: subsoiling)</t>
   </si>
   <si>
@@ -1307,9 +1295,6 @@
     <t>47 a. If yes, please describe tillage.</t>
   </si>
   <si>
-    <t>48. How much total Nitrogen fertilizer will this year's crop receive?</t>
-  </si>
-  <si>
     <t>Are there other considerations or things you want us to know about this field? (why you plant cover crops there, it stays very wet, it's generally high biomass, it's new to cover crops, etc.)</t>
   </si>
   <si>
@@ -1317,6 +1302,69 @@
   </si>
   <si>
     <t>1. State farm is located [please enter the two-letter abbreviation for your state, example: NC]</t>
+  </si>
+  <si>
+    <t>grain_sorghum</t>
+  </si>
+  <si>
+    <t>Grain Sorghum</t>
+  </si>
+  <si>
+    <t>silage_corn</t>
+  </si>
+  <si>
+    <t>Silage Corn</t>
+  </si>
+  <si>
+    <t>Wheat (winter)</t>
+  </si>
+  <si>
+    <t>wheat_spring</t>
+  </si>
+  <si>
+    <t>wheat_winter</t>
+  </si>
+  <si>
+    <t>Wheat (spring)</t>
+  </si>
+  <si>
+    <t>cover_crop_rotation</t>
+  </si>
+  <si>
+    <t>13. Have you planted COVER CROPS every consecutive year since?</t>
+  </si>
+  <si>
+    <t>13 a. If no, describe your cover crop rotation.</t>
+  </si>
+  <si>
+    <t>select_mulitple sv07f73</t>
+  </si>
+  <si>
+    <t>nfert_rate_plus_manure</t>
+  </si>
+  <si>
+    <t>the above rate plus manure</t>
+  </si>
+  <si>
+    <t>select_multiple sv07f73</t>
+  </si>
+  <si>
+    <t>48. How much total Nitrogen fertilizer will this year's crop receive? (if you already selected that the COVER CROP received litter or manure, do not add it again here)</t>
+  </si>
+  <si>
+    <t>39. Do you apply litter, manure or fertility to your COVER CROP?</t>
+  </si>
+  <si>
+    <t>Timeframe from cover crop planting to a month before crop planting.</t>
+  </si>
+  <si>
+    <t>31. What crops are GENERALLY in your crop rotation for this field?</t>
+  </si>
+  <si>
+    <t>winter_cover</t>
+  </si>
+  <si>
+    <t>Winter Cover Crop</t>
   </si>
 </sst>
 </file>
@@ -1658,10 +1706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103:XFD103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1794,7 +1842,7 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -1813,7 +1861,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
@@ -1822,7 +1870,7 @@
         <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1830,7 +1878,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
@@ -1839,7 +1887,7 @@
         <v>15</v>
       </c>
       <c r="H12" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1847,7 +1895,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C13" t="s">
         <v>31</v>
@@ -1856,7 +1904,7 @@
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1864,7 +1912,7 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
@@ -1873,7 +1921,7 @@
         <v>15</v>
       </c>
       <c r="H14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1881,16 +1929,16 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C15" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1898,7 +1946,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C16" t="s">
         <v>33</v>
@@ -1907,7 +1955,7 @@
         <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1915,7 +1963,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
@@ -1949,7 +1997,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="E19" t="b">
         <v>1</v>
@@ -2173,7 +2221,7 @@
         <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>436</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
@@ -2181,58 +2229,55 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>435</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" t="s">
-        <v>15</v>
+        <v>437</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E37" t="s">
         <v>15</v>
-      </c>
-      <c r="H37" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
+      </c>
+      <c r="H38" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
@@ -2240,132 +2285,129 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
-      </c>
-      <c r="H40" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
+      </c>
+      <c r="H41" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
-      </c>
-      <c r="H42" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C43" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
+      </c>
+      <c r="H43" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E44" t="s">
         <v>15</v>
-      </c>
-      <c r="H44" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
       </c>
       <c r="H45" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C46" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
       </c>
       <c r="H46" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C47" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
       </c>
       <c r="H47" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
@@ -2373,95 +2415,98 @@
         <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C48" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E48" t="s">
         <v>15</v>
+      </c>
+      <c r="H48" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C49" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E49" t="s">
         <v>15</v>
-      </c>
-      <c r="H49" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="B50" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C50" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E50" t="s">
         <v>15</v>
       </c>
       <c r="H50" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C51" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E51" t="s">
         <v>15</v>
       </c>
       <c r="H51" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B52" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C52" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E52" t="s">
         <v>15</v>
       </c>
       <c r="H52" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C53" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>
+      </c>
+      <c r="H53" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
@@ -2469,10 +2514,10 @@
         <v>37</v>
       </c>
       <c r="B54" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C54" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E54" t="s">
         <v>15</v>
@@ -2483,10 +2528,10 @@
         <v>37</v>
       </c>
       <c r="B55" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E55" t="s">
         <v>15</v>
@@ -2497,10 +2542,10 @@
         <v>37</v>
       </c>
       <c r="B56" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C56" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E56" t="s">
         <v>15</v>
@@ -2511,10 +2556,10 @@
         <v>37</v>
       </c>
       <c r="B57" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C57" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E57" t="s">
         <v>15</v>
@@ -2522,13 +2567,13 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C58" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E58" t="s">
         <v>15</v>
@@ -2536,13 +2581,13 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="B59" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C59" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E59" t="s">
         <v>15</v>
@@ -2553,10 +2598,10 @@
         <v>37</v>
       </c>
       <c r="B60" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
@@ -2564,13 +2609,13 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B61" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C61" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E61" t="s">
         <v>15</v>
@@ -2578,77 +2623,77 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>28</v>
+        <v>17</v>
+      </c>
+      <c r="B62" t="s">
+        <v>138</v>
+      </c>
+      <c r="C62" t="s">
+        <v>139</v>
+      </c>
+      <c r="E62" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>141</v>
-      </c>
-      <c r="B63" t="s">
-        <v>142</v>
-      </c>
-      <c r="C63" t="s">
-        <v>143</v>
-      </c>
-      <c r="E63" t="s">
-        <v>15</v>
-      </c>
-      <c r="F63" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="B64" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C64" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E64" t="s">
         <v>15</v>
+      </c>
+      <c r="F64" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C65" t="s">
-        <v>380</v>
-      </c>
-      <c r="E65" t="b">
-        <v>1</v>
+        <v>144</v>
+      </c>
+      <c r="E65" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>147</v>
+        <v>37</v>
       </c>
       <c r="B66" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C66" t="s">
-        <v>381</v>
-      </c>
-      <c r="E66" t="s">
-        <v>15</v>
+        <v>378</v>
+      </c>
+      <c r="E66" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>146</v>
       </c>
       <c r="B67" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C67" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E67" t="s">
         <v>15</v>
@@ -2656,13 +2701,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>150</v>
+        <v>72</v>
       </c>
       <c r="B68" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C68" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E68" t="s">
         <v>15</v>
@@ -2670,13 +2715,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>60</v>
+        <v>149</v>
       </c>
       <c r="B69" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C69" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E69" t="s">
         <v>15</v>
@@ -2684,13 +2729,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>153</v>
+        <v>60</v>
       </c>
       <c r="B70" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C70" t="s">
-        <v>385</v>
+        <v>445</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
@@ -2698,13 +2743,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B71" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C71" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E71" t="s">
         <v>15</v>
@@ -2712,16 +2757,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>157</v>
+        <v>438</v>
       </c>
       <c r="B72" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C72" t="s">
-        <v>387</v>
-      </c>
-      <c r="D72" t="s">
-        <v>159</v>
+        <v>383</v>
       </c>
       <c r="E72" t="s">
         <v>15</v>
@@ -2729,13 +2771,16 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B73" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C73" t="s">
-        <v>388</v>
+        <v>384</v>
+      </c>
+      <c r="D73" t="s">
+        <v>157</v>
       </c>
       <c r="E73" t="s">
         <v>15</v>
@@ -2743,13 +2788,13 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B74" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C74" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E74" t="s">
         <v>15</v>
@@ -2757,13 +2802,13 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="B75" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C75" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="E75" t="s">
         <v>15</v>
@@ -2771,13 +2816,13 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>165</v>
+        <v>57</v>
       </c>
       <c r="B76" t="s">
-        <v>392</v>
+        <v>162</v>
       </c>
       <c r="C76" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="E76" t="s">
         <v>15</v>
@@ -2785,19 +2830,16 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="B77" t="s">
-        <v>410</v>
+        <v>389</v>
       </c>
       <c r="C77" t="s">
-        <v>407</v>
+        <v>388</v>
       </c>
       <c r="E77" t="s">
         <v>15</v>
-      </c>
-      <c r="H77" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
@@ -2805,16 +2847,16 @@
         <v>57</v>
       </c>
       <c r="B78" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C78" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="E78" t="s">
         <v>15</v>
       </c>
       <c r="H78" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
@@ -2822,16 +2864,16 @@
         <v>57</v>
       </c>
       <c r="B79" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C79" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="E79" t="s">
         <v>15</v>
       </c>
       <c r="H79" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
@@ -2839,16 +2881,16 @@
         <v>57</v>
       </c>
       <c r="B80" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C80" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="E80" t="s">
         <v>15</v>
       </c>
       <c r="H80" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
@@ -2856,16 +2898,16 @@
         <v>57</v>
       </c>
       <c r="B81" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C81" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="E81" t="s">
         <v>15</v>
       </c>
       <c r="H81" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
@@ -2873,7 +2915,7 @@
         <v>57</v>
       </c>
       <c r="B82" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C82" t="s">
         <v>405</v>
@@ -2882,7 +2924,7 @@
         <v>15</v>
       </c>
       <c r="H82" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.35">
@@ -2890,58 +2932,64 @@
         <v>57</v>
       </c>
       <c r="B83" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C83" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
       </c>
       <c r="H83" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B84" t="s">
-        <v>393</v>
+        <v>413</v>
       </c>
       <c r="C84" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="E84" t="s">
         <v>15</v>
       </c>
       <c r="H84" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B85" t="s">
-        <v>166</v>
+        <v>390</v>
       </c>
       <c r="C85" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="E85" t="s">
         <v>15</v>
+      </c>
+      <c r="H85" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B86" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C86" t="s">
-        <v>418</v>
+        <v>443</v>
+      </c>
+      <c r="D86" t="s">
+        <v>444</v>
       </c>
       <c r="E86" t="s">
         <v>15</v>
@@ -2949,44 +2997,44 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="B87" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C87" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
-      </c>
-      <c r="H87" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>170</v>
+        <v>37</v>
       </c>
       <c r="B88" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C88" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
+      </c>
+      <c r="H88" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B89" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C89" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="E89" t="s">
         <v>15</v>
@@ -2994,13 +3042,13 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>57</v>
+        <v>170</v>
       </c>
       <c r="B90" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C90" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="E90" t="s">
         <v>15</v>
@@ -3008,16 +3056,13 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>175</v>
+        <v>57</v>
       </c>
       <c r="B91" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C91" t="s">
-        <v>423</v>
-      </c>
-      <c r="D91" t="s">
-        <v>177</v>
+        <v>418</v>
       </c>
       <c r="E91" t="s">
         <v>15</v>
@@ -3025,13 +3070,16 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>37</v>
+        <v>173</v>
       </c>
       <c r="B92" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C92" t="s">
-        <v>424</v>
+        <v>419</v>
+      </c>
+      <c r="D92" t="s">
+        <v>175</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
@@ -3042,10 +3090,10 @@
         <v>37</v>
       </c>
       <c r="B93" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C93" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="E93" t="s">
         <v>15</v>
@@ -3053,61 +3101,61 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B94" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C94" t="s">
-        <v>426</v>
-      </c>
-      <c r="D94" t="s">
-        <v>181</v>
-      </c>
-      <c r="E94" t="b">
-        <v>1</v>
+        <v>421</v>
+      </c>
+      <c r="E94" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="B95" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C95" t="s">
-        <v>427</v>
+        <v>422</v>
+      </c>
+      <c r="D95" t="s">
+        <v>179</v>
       </c>
       <c r="E95" t="b">
         <v>1</v>
       </c>
-      <c r="H95" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>155</v>
+        <v>37</v>
       </c>
       <c r="B96" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C96" t="s">
-        <v>428</v>
-      </c>
-      <c r="E96" t="s">
-        <v>15</v>
+        <v>423</v>
+      </c>
+      <c r="E96" t="b">
+        <v>1</v>
+      </c>
+      <c r="H96" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>37</v>
+        <v>441</v>
       </c>
       <c r="B97" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C97" t="s">
-        <v>429</v>
+        <v>442</v>
       </c>
       <c r="E97" t="s">
         <v>15</v>
@@ -3115,13 +3163,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B98" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C98" t="s">
-        <v>187</v>
+        <v>424</v>
       </c>
       <c r="E98" t="s">
         <v>15</v>
@@ -3129,21 +3177,21 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>188</v>
+        <v>17</v>
+      </c>
+      <c r="B99" t="s">
+        <v>184</v>
+      </c>
+      <c r="C99" t="s">
+        <v>185</v>
+      </c>
+      <c r="E99" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>17</v>
-      </c>
-      <c r="B100" t="s">
-        <v>189</v>
-      </c>
-      <c r="C100" t="s">
-        <v>190</v>
-      </c>
-      <c r="E100" t="s">
-        <v>15</v>
+        <v>186</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
@@ -3151,10 +3199,10 @@
         <v>17</v>
       </c>
       <c r="B101" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C101" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E101" t="s">
         <v>15</v>
@@ -3165,12 +3213,26 @@
         <v>17</v>
       </c>
       <c r="B102" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C102" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E102" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>17</v>
+      </c>
+      <c r="B103" t="s">
+        <v>191</v>
+      </c>
+      <c r="C103" t="s">
+        <v>192</v>
+      </c>
+      <c r="E103" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3181,10 +3243,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C94"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3194,7 +3256,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3205,1025 +3267,1091 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" t="s">
         <v>196</v>
-      </c>
-      <c r="B2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" t="s">
         <v>201</v>
-      </c>
-      <c r="B4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C4" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6" t="s">
         <v>206</v>
-      </c>
-      <c r="B6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C6" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B7" t="s">
-        <v>209</v>
+        <v>429</v>
       </c>
       <c r="C7" t="s">
-        <v>210</v>
+        <v>430</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C8" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B9" t="s">
-        <v>213</v>
+        <v>433</v>
       </c>
       <c r="C9" t="s">
-        <v>214</v>
+        <v>431</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B10" t="s">
-        <v>215</v>
+        <v>432</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>434</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B11" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C11" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B12" t="s">
-        <v>219</v>
+        <v>427</v>
       </c>
       <c r="C12" t="s">
-        <v>220</v>
+        <v>428</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B13" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C13" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B14" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C14" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B15" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C15" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B16" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C16" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B17" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C17" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B18" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C18" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B19" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C19" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="B20" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C20" t="s">
-        <v>198</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="B21" t="s">
-        <v>237</v>
+        <v>446</v>
       </c>
       <c r="C21" t="s">
-        <v>200</v>
+        <v>447</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="B22" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
       <c r="C22" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="B23" t="s">
-        <v>199</v>
+        <v>231</v>
       </c>
       <c r="C23" t="s">
-        <v>200</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B24" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C24" t="s">
-        <v>241</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B25" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C25" t="s">
-        <v>243</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B26" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="C26" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B27" t="s">
-        <v>244</v>
+        <v>197</v>
       </c>
       <c r="C27" t="s">
-        <v>245</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>237</v>
+      </c>
+      <c r="B28" t="s">
+        <v>238</v>
+      </c>
+      <c r="C28" t="s">
         <v>239</v>
-      </c>
-      <c r="B28" t="s">
-        <v>246</v>
-      </c>
-      <c r="C28" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B29" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C29" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B30" t="s">
-        <v>250</v>
+        <v>209</v>
       </c>
       <c r="C30" t="s">
-        <v>251</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B31" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="C31" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B32" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C32" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B33" t="s">
-        <v>256</v>
+        <v>217</v>
       </c>
       <c r="C33" t="s">
-        <v>257</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B34" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="C34" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B35" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="C35" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B36" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="C36" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B37" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="C37" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B38" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="C38" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B39" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="C39" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B40" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="C40" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B41" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="C41" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B42" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="C42" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B43" t="s">
-        <v>233</v>
+        <v>264</v>
       </c>
       <c r="C43" t="s">
-        <v>234</v>
+        <v>265</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>276</v>
+        <v>237</v>
       </c>
       <c r="B44" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="C44" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>276</v>
+        <v>237</v>
       </c>
       <c r="B45" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="C45" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>276</v>
+        <v>237</v>
       </c>
       <c r="B46" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="C46" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>283</v>
+        <v>237</v>
       </c>
       <c r="B47" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="C47" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>283</v>
+        <v>237</v>
       </c>
       <c r="B48" t="s">
-        <v>286</v>
+        <v>231</v>
       </c>
       <c r="C48" t="s">
-        <v>287</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B49" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="C49" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B50" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="C50" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B51" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="C51" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>281</v>
+      </c>
+      <c r="B52" t="s">
+        <v>282</v>
+      </c>
+      <c r="C52" t="s">
         <v>283</v>
-      </c>
-      <c r="B52" t="s">
-        <v>294</v>
-      </c>
-      <c r="C52" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B53" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="C53" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B54" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="C54" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="B55" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="C55" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="B56" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="C56" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="B57" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="C57" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="B58" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="C58" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="B59" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="C59" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="B60" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="C60" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="B61" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="C61" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B62" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C62" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>303</v>
+      </c>
+      <c r="B63" t="s">
         <v>305</v>
       </c>
-      <c r="B63" t="s">
-        <v>317</v>
-      </c>
       <c r="C63" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B64" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="C64" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="B65" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="C65" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="B66" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="C66" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="B67" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="C67" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="B68" t="s">
-        <v>233</v>
+        <v>315</v>
       </c>
       <c r="C68" t="s">
-        <v>234</v>
+        <v>316</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>328</v>
+        <v>303</v>
       </c>
       <c r="B69" t="s">
-        <v>394</v>
+        <v>317</v>
       </c>
       <c r="C69" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>328</v>
+        <v>303</v>
       </c>
       <c r="B70" t="s">
-        <v>395</v>
+        <v>439</v>
       </c>
       <c r="C70" t="s">
-        <v>330</v>
+        <v>440</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B71" t="s">
-        <v>396</v>
+        <v>320</v>
       </c>
       <c r="C71" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B72" t="s">
-        <v>397</v>
+        <v>322</v>
       </c>
       <c r="C72" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="B73" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="C73" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="B74" t="s">
-        <v>335</v>
+        <v>231</v>
       </c>
       <c r="C74" t="s">
-        <v>336</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B75" t="s">
-        <v>337</v>
+        <v>391</v>
       </c>
       <c r="C75" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="B76" t="s">
-        <v>340</v>
+        <v>392</v>
       </c>
       <c r="C76" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="B77" t="s">
-        <v>342</v>
+        <v>393</v>
       </c>
       <c r="C77" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="B78" t="s">
-        <v>344</v>
+        <v>394</v>
       </c>
       <c r="C78" t="s">
-        <v>345</v>
+        <v>232</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="B79" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="C79" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="B80" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="C80" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="B81" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="C81" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>337</v>
+      </c>
+      <c r="B82" t="s">
+        <v>338</v>
+      </c>
+      <c r="C82" t="s">
         <v>339</v>
-      </c>
-      <c r="B82" t="s">
-        <v>352</v>
-      </c>
-      <c r="C82" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B83" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="C83" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B84" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="C84" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B85" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="C85" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B86" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="C86" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B87" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="C87" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B88" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="C88" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B89" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="C89" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B90" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="C90" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B91" t="s">
-        <v>233</v>
+        <v>356</v>
       </c>
       <c r="C91" t="s">
-        <v>234</v>
+        <v>357</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>370</v>
+        <v>337</v>
       </c>
       <c r="B92" t="s">
-        <v>207</v>
+        <v>358</v>
       </c>
       <c r="C92" t="s">
-        <v>208</v>
+        <v>359</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>370</v>
+        <v>337</v>
       </c>
       <c r="B93" t="s">
-        <v>209</v>
+        <v>360</v>
       </c>
       <c r="C93" t="s">
-        <v>210</v>
+        <v>361</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>370</v>
+        <v>337</v>
       </c>
       <c r="B94" t="s">
-        <v>213</v>
+        <v>362</v>
       </c>
       <c r="C94" t="s">
-        <v>214</v>
+        <v>363</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>337</v>
+      </c>
+      <c r="B95" t="s">
+        <v>364</v>
+      </c>
+      <c r="C95" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>337</v>
+      </c>
+      <c r="B96" t="s">
+        <v>366</v>
+      </c>
+      <c r="C96" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>337</v>
+      </c>
+      <c r="B97" t="s">
+        <v>231</v>
+      </c>
+      <c r="C97" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>368</v>
+      </c>
+      <c r="B98" t="s">
+        <v>205</v>
+      </c>
+      <c r="C98" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>368</v>
+      </c>
+      <c r="B99" t="s">
+        <v>207</v>
+      </c>
+      <c r="C99" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>368</v>
+      </c>
+      <c r="B100" t="s">
+        <v>211</v>
+      </c>
+      <c r="C100" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>